<commit_message>
finished up pg utils
</commit_message>
<xml_diff>
--- a/packages/pg/tests/test-pg-data-loading.xlsx
+++ b/packages/pg/tests/test-pg-data-loading.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Documents/sentosa/code/stcland/packages/pg/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C05B6D-4D15-ED42-BFCB-325EDAAA69B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2904B8C9-3727-F445-8846-08D8165E98B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23200" yWindow="500" windowWidth="68580" windowHeight="24140" activeTab="6" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19440" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="9" r:id="rId1"/>
@@ -23,19 +23,16 @@
     <sheet name=".enums" sheetId="17" r:id="rId8"/>
     <sheet name=".lists" sheetId="7" r:id="rId9"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId10"/>
-  </externalReferences>
   <definedNames>
-    <definedName name="_Action">'[1].enums'!$I$2:$I$6</definedName>
+    <definedName name="_Action">'.enums'!$I$2:$I$6</definedName>
     <definedName name="_Actions">'.enums'!$I$2:$I$6</definedName>
     <definedName name="_GameFormats">'.enums'!$E$2:$E$3</definedName>
     <definedName name="_GameTypes">'.enums'!$D$2:$D$3</definedName>
-    <definedName name="_Position">'[1].enums'!$C$2:$C$11</definedName>
+    <definedName name="_Position">'.enums'!$C$2:$C$11</definedName>
     <definedName name="_Positions">'.enums'!$C$2:$C$11</definedName>
     <definedName name="_Roles">'.enums'!$A$2:$A$4</definedName>
     <definedName name="_SeatNums">'.enums'!$B$2:$B$11</definedName>
-    <definedName name="_Street">'[1].enums'!$H$2:$H$5</definedName>
+    <definedName name="_Street">'.enums'!$H$2:$H$5</definedName>
     <definedName name="_Streets">'.enums'!$H$2:$H$5</definedName>
     <definedName name="_VenueTypes">'.enums'!$F$2:$F$3</definedName>
     <definedName name="Currencies">'.enums'!$G$2:$G$4</definedName>
@@ -223,9 +220,6 @@
     <t>NL50</t>
   </si>
   <si>
-    <t>isCustom</t>
-  </si>
-  <si>
     <t>First Table Ever</t>
   </si>
   <si>
@@ -536,6 +530,9 @@
   </si>
   <si>
     <t>stack_remaining</t>
+  </si>
+  <si>
+    <t>is_custom</t>
   </si>
 </sst>
 </file>
@@ -720,7 +717,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -769,46 +766,43 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -826,120 +820,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="dUsers"/>
-      <sheetName val="dPlayers"/>
-      <sheetName val="dCashStakes"/>
-      <sheetName val="dVenues"/>
-      <sheetName val="dHands"/>
-      <sheetName val="dHandActions"/>
-      <sheetName val="ePlayersToHands"/>
-      <sheetName val="eHandSequences"/>
-      <sheetName val="gHandsGraph"/>
-      <sheetName val=".enums"/>
-      <sheetName val=".iists"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9">
-        <row r="2">
-          <cell r="C2" t="str">
-            <v>BB</v>
-          </cell>
-          <cell r="H2" t="str">
-            <v>PRE_FLOP</v>
-          </cell>
-          <cell r="I2" t="str">
-            <v>CHECK</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="C3" t="str">
-            <v>SB</v>
-          </cell>
-          <cell r="H3" t="str">
-            <v>FLOP</v>
-          </cell>
-          <cell r="I3" t="str">
-            <v>CALL</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="C4" t="str">
-            <v>UTG</v>
-          </cell>
-          <cell r="H4" t="str">
-            <v>TURN</v>
-          </cell>
-          <cell r="I4" t="str">
-            <v>BET</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="C5" t="str">
-            <v>UTG+1</v>
-          </cell>
-          <cell r="H5" t="str">
-            <v>RIVER</v>
-          </cell>
-          <cell r="I5" t="str">
-            <v>RAISE</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="C6" t="str">
-            <v>UTG+2</v>
-          </cell>
-          <cell r="I6" t="str">
-            <v>FOLD</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="C7" t="str">
-            <v>UTG+3</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="C8" t="str">
-            <v>LJ</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="C9" t="str">
-            <v>HJ</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="C10" t="str">
-            <v>CO</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="C11" t="str">
-            <v>BTN</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="10"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1241,8 +1121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0992D42-8EDD-1644-B63D-73C3203972BD}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1287,7 +1167,7 @@
     </row>
     <row r="5" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>1</v>
@@ -1301,7 +1181,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>30</v>
@@ -1315,7 +1195,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>33</v>
@@ -1375,7 +1255,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1419,7 +1299,7 @@
         <v>8</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>53</v>
+        <v>157</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>50</v>
@@ -1427,7 +1307,7 @@
     </row>
     <row r="5" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>0</v>
@@ -1447,7 +1327,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
@@ -1467,7 +1347,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B7" s="2">
         <v>2</v>
@@ -1487,7 +1367,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B8" s="2">
         <v>100</v>
@@ -1496,7 +1376,7 @@
         <v>200</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E8" s="2" t="b">
         <v>0</v>
@@ -1507,7 +1387,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B9" s="2">
         <v>0.1</v>
@@ -1527,7 +1407,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B10" s="2">
         <v>0.25</v>
@@ -1586,7 +1466,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1631,10 +1511,10 @@
     </row>
     <row r="5" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>73</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>74</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>1</v>
@@ -1645,10 +1525,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>35</v>
@@ -1659,10 +1539,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>37</v>
@@ -1673,10 +1553,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>116</v>
-      </c>
-      <c r="B8" s="37" t="s">
-        <v>145</v>
+        <v>115</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>144</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>39</v>
@@ -1687,10 +1567,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>117</v>
-      </c>
-      <c r="B9" s="37" t="s">
-        <v>145</v>
+        <v>116</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>144</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>40</v>
@@ -1701,10 +1581,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>146</v>
-      </c>
-      <c r="B10" s="37" t="s">
         <v>145</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>144</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>43</v>
@@ -1754,7 +1634,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1792,18 +1672,18 @@
         <v>8</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>1</v>
@@ -1812,7 +1692,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>0</v>
@@ -1820,16 +1700,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E6" s="2">
         <v>6</v>
@@ -1888,7 +1768,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1922,30 +1802,30 @@
     </row>
     <row r="4" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="D4" s="7" t="s">
+      <c r="F4" s="5" t="s">
         <v>137</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>73</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>74</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>0</v>
@@ -1962,10 +1842,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -1977,7 +1857,7 @@
         <v>300</v>
       </c>
       <c r="F6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -2062,7 +1942,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2100,39 +1980,39 @@
         <v>23</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="F4" s="7" t="s">
+      <c r="G4" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="H4" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="I4" s="7" t="s">
         <v>65</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>74</v>
-      </c>
       <c r="C5" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>0</v>
@@ -2155,22 +2035,22 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" t="s">
         <v>69</v>
-      </c>
-      <c r="F6" t="s">
-        <v>70</v>
       </c>
       <c r="G6">
         <v>1000000</v>
@@ -2184,22 +2064,22 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D7" s="2">
         <v>3</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G7">
         <v>1500000</v>
@@ -2213,22 +2093,22 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D8" s="2">
         <v>4</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G8">
         <v>800000</v>
@@ -2296,10 +2176,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{490F7804-6FAB-AC46-A3F8-9390691D26BA}">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2313,9 +2193,10 @@
     <col min="7" max="7" width="18.5" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" customWidth="1"/>
     <col min="9" max="10" width="19.33203125" customWidth="1"/>
+    <col min="11" max="11" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>12</v>
       </c>
@@ -2323,60 +2204,60 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="H4" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="I4" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="J4" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="K4" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="J4" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>1</v>
@@ -2403,589 +2284,574 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" s="22" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="22" t="s">
-        <v>121</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="E6" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="F6" s="22">
+      <c r="B6" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="21">
         <v>1</v>
       </c>
-      <c r="G6" s="22">
+      <c r="G6" s="21">
         <v>300</v>
       </c>
-      <c r="H6" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="I6" s="22">
+      <c r="H6" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="I6" s="21">
         <v>500</v>
       </c>
-      <c r="J6" s="22" t="b">
-        <v>0</v>
-      </c>
-      <c r="K6" s="22">
+      <c r="J6" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6" s="29">
         <f>hand_players!G6-hand_actions!I6</f>
         <v>999500</v>
       </c>
-      <c r="L6" s="23"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="B7" s="20" t="s">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="F7" s="20">
+      <c r="B7" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7" s="30">
         <f>F6+1</f>
         <v>2</v>
       </c>
-      <c r="G7" s="20">
+      <c r="G7" s="30">
         <f>G6+I6</f>
         <v>800</v>
       </c>
-      <c r="H7" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="I7" s="20">
+      <c r="H7" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="I7" s="30">
         <v>500</v>
       </c>
-      <c r="J7" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="K7" s="20">
+      <c r="J7" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" s="31">
         <f>hand_players!G7-hand_actions!I7</f>
         <v>1499500</v>
       </c>
-      <c r="L7" s="25"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="B8" s="27" t="s">
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="C8" s="27" t="s">
-        <v>123</v>
-      </c>
-      <c r="D8" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="E8" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="F8" s="27">
+      <c r="B8" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="F8" s="24">
         <f t="shared" ref="F8:F19" si="0">F7+1</f>
         <v>3</v>
       </c>
-      <c r="G8" s="27">
+      <c r="G8" s="24">
         <f>G7+I7</f>
         <v>1300</v>
       </c>
-      <c r="H8" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="I8" s="27">
+      <c r="H8" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="I8" s="24">
         <v>500</v>
       </c>
-      <c r="J8" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="K8" s="27">
+      <c r="J8" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" s="32">
         <f>hand_players!G8-hand_actions!I8</f>
         <v>799500</v>
       </c>
-      <c r="L8" s="28"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="B9" s="22" t="s">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="C9" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="D9" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="E9" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="F9" s="22">
+      <c r="B9" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="F9" s="21">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G9" s="22">
-        <f t="shared" ref="G9:G20" si="1">G8+I8</f>
+      <c r="G9" s="21">
+        <f>G8+I8</f>
         <v>1800</v>
       </c>
-      <c r="H9" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="I9" s="22">
-        <v>0</v>
-      </c>
-      <c r="J9" s="22" t="b">
-        <v>0</v>
-      </c>
-      <c r="K9" s="22">
+      <c r="H9" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="I9" s="21">
+        <v>0</v>
+      </c>
+      <c r="J9" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" s="29">
         <f>K6-I9</f>
         <v>999500</v>
       </c>
-      <c r="L9" s="23"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="B10" s="20" t="s">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="C10" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="D10" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="E10" s="31" t="s">
-        <v>93</v>
-      </c>
-      <c r="F10" s="20">
+      <c r="B10" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="F10" s="30">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G10" s="20">
-        <f t="shared" si="1"/>
+      <c r="G10" s="30">
+        <f>G9+I9</f>
         <v>1800</v>
       </c>
-      <c r="H10" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="I10" s="20">
-        <v>0</v>
-      </c>
-      <c r="J10" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="K10" s="20">
+      <c r="H10" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I10" s="30">
+        <v>0</v>
+      </c>
+      <c r="J10" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="K10" s="31">
         <f>K7-I10</f>
         <v>1499500</v>
       </c>
-      <c r="L10" s="25"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="B11" s="27" t="s">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="C11" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="D11" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="E11" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="F11" s="27">
+      <c r="B11" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="F11" s="24">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G11" s="27">
-        <f t="shared" si="1"/>
+      <c r="G11" s="24">
+        <f>G10+I10</f>
         <v>1800</v>
       </c>
-      <c r="H11" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="I11" s="27">
-        <v>0</v>
-      </c>
-      <c r="J11" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="K11" s="27">
+      <c r="H11" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="I11" s="24">
+        <v>0</v>
+      </c>
+      <c r="J11" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11" s="32">
         <f>K8-I11</f>
         <v>799500</v>
       </c>
-      <c r="L11" s="28"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="B12" s="22" t="s">
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="C12" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="D12" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="E12" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="F12" s="22">
+      <c r="B12" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="F12" s="21">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="G12" s="22">
-        <f t="shared" si="1"/>
+      <c r="G12" s="21">
+        <f>G11+I11</f>
         <v>1800</v>
       </c>
-      <c r="H12" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="I12" s="22">
-        <v>0</v>
-      </c>
-      <c r="J12" s="22" t="b">
-        <v>0</v>
-      </c>
-      <c r="K12" s="22">
+      <c r="H12" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="I12" s="21">
+        <v>0</v>
+      </c>
+      <c r="J12" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" s="29">
         <f>K9</f>
         <v>999500</v>
       </c>
-      <c r="L12" s="23"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="B13" s="20" t="s">
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="C13" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="D13" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="F13" s="20">
+      <c r="B13" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="F13" s="30">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="G13" s="20">
-        <f t="shared" si="1"/>
+      <c r="G13" s="30">
+        <f>G12+I12</f>
         <v>1800</v>
       </c>
-      <c r="H13" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="I13" s="20">
-        <v>0</v>
-      </c>
-      <c r="J13" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="K13" s="20">
+      <c r="H13" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I13" s="30">
+        <v>0</v>
+      </c>
+      <c r="J13" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" s="31">
         <f>K10</f>
         <v>1499500</v>
       </c>
-      <c r="L13" s="25"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="B14" s="20" t="s">
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="C14" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="D14" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="F14" s="20">
+      <c r="B14" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="F14" s="30">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="G14" s="20">
-        <f t="shared" si="1"/>
+      <c r="G14" s="30">
+        <f>G13+I13</f>
         <v>1800</v>
       </c>
-      <c r="H14" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="I14" s="20">
+      <c r="H14" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="I14" s="30">
         <v>1200</v>
       </c>
-      <c r="J14" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="K14" s="20">
+      <c r="J14" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" s="31">
         <f>K11-I14</f>
         <v>798300</v>
       </c>
-      <c r="L14" s="25"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="B15" s="20" t="s">
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="C15" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="D15" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="F15" s="20">
+      <c r="B15" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="F15" s="30">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G15" s="20">
-        <f t="shared" si="1"/>
+      <c r="G15" s="30">
+        <f>G14+I14</f>
         <v>3000</v>
       </c>
-      <c r="H15" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="I15" s="20">
+      <c r="H15" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="I15" s="30">
         <f>I14</f>
         <v>1200</v>
       </c>
-      <c r="J15" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="K15" s="20">
+      <c r="J15" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" s="31">
         <f>K12-I15</f>
         <v>998300</v>
       </c>
-      <c r="L15" s="25"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="B16" s="27" t="s">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="C16" s="27" t="s">
-        <v>121</v>
-      </c>
-      <c r="D16" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="E16" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="F16" s="27">
+      <c r="B16" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="F16" s="24">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="G16" s="27">
-        <f t="shared" si="1"/>
+      <c r="G16" s="24">
+        <f>G15+I15</f>
         <v>4200</v>
       </c>
-      <c r="H16" s="27" t="s">
-        <v>104</v>
-      </c>
-      <c r="I16" s="27">
-        <v>0</v>
-      </c>
-      <c r="J16" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="K16" s="27">
+      <c r="H16" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="I16" s="24">
+        <v>0</v>
+      </c>
+      <c r="J16" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16" s="32">
         <f>K13</f>
         <v>1499500</v>
       </c>
-      <c r="L16" s="28"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="B17" s="22" t="s">
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="C17" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="D17" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="F17" s="22">
+      <c r="B17" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="F17" s="21">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="G17" s="22">
-        <f t="shared" si="1"/>
+      <c r="G17" s="21">
+        <f>G16+I16</f>
         <v>4200</v>
       </c>
-      <c r="H17" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="I17" s="35">
-        <v>0</v>
-      </c>
-      <c r="J17" s="35" t="b">
-        <v>0</v>
-      </c>
-      <c r="K17" s="22">
+      <c r="H17" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="I17" s="21">
+        <v>0</v>
+      </c>
+      <c r="J17" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K17" s="29">
         <f>K15</f>
         <v>998300</v>
       </c>
-      <c r="L17" s="23"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="B18" s="20" t="s">
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="C18" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="D18" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="F18" s="20">
+      <c r="B18" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="D18" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="F18" s="30">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="G18" s="20">
-        <f t="shared" si="1"/>
+      <c r="G18" s="30">
+        <f>G17+I17</f>
         <v>4200</v>
       </c>
-      <c r="H18" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="I18" s="34">
+      <c r="H18" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="I18" s="30">
         <v>1200</v>
       </c>
-      <c r="J18" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="K18" s="20">
+      <c r="J18" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="K18" s="31">
         <f>K14-I18</f>
         <v>797100</v>
       </c>
-      <c r="L18" s="25"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="B19" s="20" t="s">
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="C19" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="D19" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="F19" s="20">
+      <c r="B19" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="D19" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="F19" s="30">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="G19" s="20">
-        <f t="shared" si="1"/>
+      <c r="G19" s="30">
+        <f>G18+I18</f>
         <v>5400</v>
       </c>
-      <c r="H19" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="I19" s="34">
+      <c r="H19" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="I19" s="30">
         <f>K17</f>
         <v>998300</v>
       </c>
-      <c r="J19" s="20" t="b">
+      <c r="J19" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="K19" s="20">
-        <v>0</v>
-      </c>
-      <c r="L19" s="25"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="B20" s="27" t="s">
+      <c r="K19" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="C20" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="D20" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="E20" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="F20" s="27">
-        <f t="shared" ref="F20" si="2">F19+1</f>
+      <c r="B20" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="D20" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="F20" s="24">
+        <f t="shared" ref="F20" si="1">F19+1</f>
         <v>15</v>
       </c>
-      <c r="G20" s="27">
-        <f t="shared" si="1"/>
+      <c r="G20" s="24">
+        <f>G19+I19</f>
         <v>1003700</v>
       </c>
-      <c r="H20" s="27" t="s">
-        <v>104</v>
-      </c>
-      <c r="I20" s="36">
-        <v>0</v>
-      </c>
-      <c r="J20" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="K20" s="27">
+      <c r="H20" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="I20" s="24">
+        <v>0</v>
+      </c>
+      <c r="J20" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="K20" s="32">
         <f>K18</f>
         <v>797100</v>
       </c>
-      <c r="L20" s="28"/>
     </row>
   </sheetData>
   <dataValidations count="7">
@@ -2996,10 +2862,7 @@
       <formula1>_Streets</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H6:H20" xr:uid="{183D1F80-CC1F-D341-A5C9-B55B214ED81E}">
-      <formula1>_Action</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:K5" xr:uid="{D439AD26-78D3-8049-B803-91FB77A799E5}">
-      <formula1>TableDataTypes</formula1>
+      <formula1>_Actions</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5" xr:uid="{ED2E2930-6163-1949-AC52-44DA18154BD8}">
       <formula1>"_Actions"</formula1>
@@ -3009,6 +2872,9 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10:D11 D13:D14 D16 D18 D20" xr:uid="{3F75985B-33E3-764E-88DD-3E88CC35A29E}">
       <formula1>_Position</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:K5" xr:uid="{D439AD26-78D3-8049-B803-91FB77A799E5}">
+      <formula1>TableDataTypes</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3033,112 +2899,112 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="D1" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="E1" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="F1" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="G1" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="H1" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="I1" s="17" t="s">
         <v>131</v>
-      </c>
-      <c r="I1" s="17" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" s="19">
         <v>1</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E2" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>83</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>84</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>51</v>
       </c>
       <c r="H2" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="I2" s="10" t="s">
         <v>85</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" s="19">
         <v>2</v>
       </c>
       <c r="C3" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="E3" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="F3" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="G3" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="H3" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="I3" s="10" t="s">
         <v>93</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" s="19">
         <v>3</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
       <c r="G4" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="H4" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="I4" s="10" t="s">
         <v>98</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -3147,17 +3013,17 @@
         <v>4</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="H5" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="I5" s="10" t="s">
         <v>101</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -3166,7 +3032,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -3174,7 +3040,7 @@
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -3183,7 +3049,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -3198,7 +3064,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -3213,7 +3079,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -3228,7 +3094,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -3243,7 +3109,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -3350,7 +3216,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9" t="s">
         <v>13</v>
@@ -3358,7 +3224,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
@@ -3391,12 +3257,12 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data loader coming along nicely
</commit_message>
<xml_diff>
--- a/packages/pg/tests/test-pg-data-loading.xlsx
+++ b/packages/pg/tests/test-pg-data-loading.xlsx
@@ -1,27 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Documents/sentosa/code/stcland/packages/pg/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2904B8C9-3727-F445-8846-08D8165E98B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA79550F-BB85-DE4D-8980-6EAF24505A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19440" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
+    <workbookView xWindow="13480" yWindow="6520" windowWidth="34560" windowHeight="19440" activeTab="3" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
   </bookViews>
   <sheets>
-    <sheet name="users" sheetId="9" r:id="rId1"/>
-    <sheet name="cash_stakes" sheetId="13" r:id="rId2"/>
-    <sheet name="players" sheetId="11" r:id="rId3"/>
-    <sheet name="tables" sheetId="12" r:id="rId4"/>
-    <sheet name="hands" sheetId="1" r:id="rId5"/>
-    <sheet name="hand_players" sheetId="15" r:id="rId6"/>
-    <sheet name="hand_actions" sheetId="16" r:id="rId7"/>
-    <sheet name=".enums" sheetId="17" r:id="rId8"/>
-    <sheet name=".lists" sheetId="7" r:id="rId9"/>
+    <sheet name="organizations" sheetId="9" r:id="rId1"/>
+    <sheet name="users" sheetId="18" r:id="rId2"/>
+    <sheet name="users_organizations" sheetId="19" r:id="rId3"/>
+    <sheet name="players" sheetId="11" r:id="rId4"/>
+    <sheet name=".tables" sheetId="12" r:id="rId5"/>
+    <sheet name=".hands" sheetId="1" r:id="rId6"/>
+    <sheet name=".hand_players" sheetId="15" r:id="rId7"/>
+    <sheet name=".hand_actions" sheetId="16" r:id="rId8"/>
+    <sheet name=".cash_stakes" sheetId="13" r:id="rId9"/>
+    <sheet name=".enums" sheetId="17" r:id="rId10"/>
+    <sheet name=".lists" sheetId="7" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_Action">'.enums'!$I$2:$I$6</definedName>
@@ -59,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="177">
   <si>
     <t>number</t>
   </si>
@@ -139,60 +141,36 @@
     <t>email</t>
   </si>
   <si>
-    <t>password_hash</t>
-  </si>
-  <si>
     <t>user_id</t>
   </si>
   <si>
     <t>nickname</t>
   </si>
   <si>
-    <t>full_name</t>
-  </si>
-  <si>
     <t>stevo</t>
   </si>
   <si>
     <t>steve@sentosatech.com</t>
   </si>
   <si>
-    <t>pw</t>
-  </si>
-  <si>
     <t>gabe</t>
   </si>
   <si>
     <t>gabe@sentosatech.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Steven Saunders </t>
-  </si>
-  <si>
     <t>Stevo</t>
   </si>
   <si>
-    <t>Gabe Alex</t>
-  </si>
-  <si>
     <t>Gabe the Crusher</t>
   </si>
   <si>
-    <t>Issac Haxton</t>
-  </si>
-  <si>
-    <t>Alex Foxen</t>
-  </si>
-  <si>
     <t>AlexF</t>
   </si>
   <si>
     <t>IkeH</t>
   </si>
   <si>
-    <t>Sean Winter</t>
-  </si>
-  <si>
     <t>SeanW</t>
   </si>
   <si>
@@ -493,9 +471,6 @@
     <t>users.u_gabe</t>
   </si>
   <si>
-    <t>_skip_</t>
-  </si>
-  <si>
     <t>p_winter:_auto_</t>
   </si>
   <si>
@@ -533,6 +508,90 @@
   </si>
   <si>
     <t>is_custom</t>
+  </si>
+  <si>
+    <t>org_tbs:_auto_</t>
+  </si>
+  <si>
+    <t>org_cpg:_auto_</t>
+  </si>
+  <si>
+    <t>Triple Barrel Software</t>
+  </si>
+  <si>
+    <t>Chacing Poker Greatness</t>
+  </si>
+  <si>
+    <t>u_brad:_auto_</t>
+  </si>
+  <si>
+    <t>brad@chasingpokergreatness.com</t>
+  </si>
+  <si>
+    <t>bradly</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>Steve</t>
+  </si>
+  <si>
+    <t>Saunders</t>
+  </si>
+  <si>
+    <t>Gabe</t>
+  </si>
+  <si>
+    <t>Alex-something</t>
+  </si>
+  <si>
+    <t>Brad</t>
+  </si>
+  <si>
+    <t>Wilson</t>
+  </si>
+  <si>
+    <t>organization_id</t>
+  </si>
+  <si>
+    <t>users.u_brad</t>
+  </si>
+  <si>
+    <t>organizations.org_tbs</t>
+  </si>
+  <si>
+    <t>organizations.org_cpg</t>
+  </si>
+  <si>
+    <t>p_brad:_auto_</t>
+  </si>
+  <si>
+    <t>Bad Brad</t>
+  </si>
+  <si>
+    <t>Isaac</t>
+  </si>
+  <si>
+    <t>Haxton</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Foxen</t>
+  </si>
+  <si>
+    <t>Sean</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>null</t>
   </si>
 </sst>
 </file>
@@ -717,7 +776,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -790,19 +849,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1119,21 +1172,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0992D42-8EDD-1644-B63D-73C3203972BD}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="38.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="29.5" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>12</v>
       </c>
@@ -1141,107 +1192,600 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
-      <c r="D14" s="9"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="15"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{0294C92A-52CF-1C4C-B799-34D896F9ADDD}">
       <formula1>DataLayouts</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:D5" xr:uid="{67FE0020-B8D4-5F4D-9F38-B9D397707CFA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:B5" xr:uid="{67FE0020-B8D4-5F4D-9F38-B9D397707CFA}">
       <formula1>TableDataTypes</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:F5" xr:uid="{64C45A4D-F67F-854C-B526-E9C071FD405F}">
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DE0DFDF-D9E5-8B47-B89F-323429675129}">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="19">
+        <v>1</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="19">
+        <v>2</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="19">
+        <v>3</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="10"/>
+      <c r="B5" s="19">
+        <v>4</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="10"/>
+      <c r="B6" s="19">
+        <v>5</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="10"/>
+      <c r="B7" s="19">
+        <v>6</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="10"/>
+      <c r="B8" s="19">
+        <v>7</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="10"/>
+      <c r="B9" s="19">
+        <v>8</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="10"/>
+      <c r="B10" s="19">
+        <v>9</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="10"/>
+      <c r="B11" s="19">
+        <v>10</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D39D9E3-0EB2-BA4D-9DA7-B5A172AB8C82}">
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BF7FE8D-D3D6-0341-A57E-3BE902F737F0}">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="38.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18" style="2" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" customWidth="1"/>
+    <col min="5" max="5" width="19.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>158</v>
+      </c>
+      <c r="E6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>160</v>
+      </c>
+      <c r="E7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="9"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="15"/>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:E5" xr:uid="{A5363200-5E32-0A4E-98B4-61E0F10BE994}">
+      <formula1>TableDataTypes</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{3277DE54-7A71-AB46-AAD9-FE82AA6DA136}">
+      <formula1>DataLayouts</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{9ED3BF64-907D-BA42-93C0-E1AF88B96F11}">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -1250,209 +1794,94 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E595855-FCC9-CD4F-A83B-9F0E43C081E7}">
-  <dimension ref="A1:F16"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EA6A974-E798-9241-8093-8124B9D0B6E3}">
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="42.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="19.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="24.83203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B6" s="2">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2">
-        <v>3</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B7" s="2">
-        <v>2</v>
-      </c>
-      <c r="C7" s="2">
-        <v>5</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B8" s="2">
-        <v>100</v>
-      </c>
-      <c r="C8" s="2">
-        <v>200</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E8" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>76</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>77</v>
-      </c>
-      <c r="B10" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E10" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
-      <c r="C12" s="9"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="15"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{3AFABB3D-38C0-CA4B-96C5-C68C5E1F75DE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{1388F5CC-5F3E-6E43-9598-EC3C28E06242}">
       <formula1>DataLayouts</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:F5" xr:uid="{2B43068A-F86C-2F43-9DA6-BD346589A1EE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:B5" xr:uid="{6BF4AD41-0577-CF45-9C61-5ACB0D6954F1}">
       <formula1>TableDataTypes</formula1>
     </dataValidation>
   </dataValidations>
@@ -1461,23 +1890,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2263EDC9-A2CB-9C45-8C08-CE3DC9B88E26}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="38.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="38.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="17.5" style="2" customWidth="1"/>
     <col min="4" max="4" width="15.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>12</v>
       </c>
@@ -1485,36 +1915,39 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>29</v>
-      </c>
       <c r="D4" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>1</v>
@@ -1522,106 +1955,141 @@
       <c r="D5" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
+        <v>158</v>
+      </c>
+      <c r="E6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>160</v>
+      </c>
+      <c r="E7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D9" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E10" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>115</v>
-      </c>
-      <c r="B8" s="28" t="s">
-        <v>144</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>116</v>
-      </c>
-      <c r="B9" s="28" t="s">
-        <v>144</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>145</v>
-      </c>
-      <c r="B10" s="28" t="s">
-        <v>144</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="9"/>
-      <c r="C12" s="9"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="15"/>
+      <c r="D11" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E11" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="9"/>
+      <c r="C13" s="9"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="15"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:D5" xr:uid="{227E0E5E-8598-1C4B-A6FF-1AF8F3D32A17}">
-      <formula1>TableDataTypes</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{F80FB675-602B-2544-8804-620039F78CFA}">
       <formula1>DataLayouts</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:E5" xr:uid="{227E0E5E-8598-1C4B-A6FF-1AF8F3D32A17}">
+      <formula1>TableDataTypes</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1629,7 +2097,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE849852-9B8D-D646-983A-87B67FBBE846}">
   <dimension ref="A1:E16"/>
   <sheetViews>
@@ -1672,18 +2140,18 @@
         <v>8</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>1</v>
@@ -1692,7 +2160,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>0</v>
@@ -1700,16 +2168,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="E6" s="2">
         <v>6</v>
@@ -1763,7 +2231,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B101DD8F-9A36-0342-BC29-1E3C3A22B2B5}">
   <dimension ref="A1:I16"/>
   <sheetViews>
@@ -1802,30 +2270,30 @@
     </row>
     <row r="4" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>0</v>
@@ -1842,10 +2310,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -1857,7 +2325,7 @@
         <v>300</v>
       </c>
       <c r="F6" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -1937,7 +2405,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D12000C3-1D3F-1248-BA35-71F90F67C3F6}">
   <dimension ref="A1:I17"/>
   <sheetViews>
@@ -1980,39 +2448,39 @@
         <v>23</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>0</v>
@@ -2035,22 +2503,22 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="F6" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="G6">
         <v>1000000</v>
@@ -2064,22 +2532,22 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D7" s="2">
         <v>3</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F7" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="G7">
         <v>1500000</v>
@@ -2093,22 +2561,22 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D8" s="2">
         <v>4</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="F8" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="G8">
         <v>800000</v>
@@ -2174,7 +2642,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{490F7804-6FAB-AC46-A3F8-9390691D26BA}">
   <dimension ref="A1:K20"/>
   <sheetViews>
@@ -2219,34 +2687,34 @@
         <v>23</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2254,10 +2722,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>1</v>
@@ -2286,19 +2754,19 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="F6" s="21">
         <v>1</v>
@@ -2307,7 +2775,7 @@
         <v>300</v>
       </c>
       <c r="H6" s="21" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="I6" s="21">
         <v>500</v>
@@ -2316,74 +2784,74 @@
         <v>0</v>
       </c>
       <c r="K6" s="29">
-        <f>hand_players!G6-hand_actions!I6</f>
+        <f>'.hand_players'!G6-'.hand_actions'!I6</f>
         <v>999500</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="C7" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="D7" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="E7" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="F7" s="30">
+        <v>72</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" s="2">
         <f>F6+1</f>
         <v>2</v>
       </c>
-      <c r="G7" s="30">
-        <f>G6+I6</f>
+      <c r="G7" s="2">
+        <f t="shared" ref="G7:G20" si="0">G6+I6</f>
         <v>800</v>
       </c>
-      <c r="H7" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="I7" s="30">
+      <c r="H7" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I7" s="2">
         <v>500</v>
       </c>
-      <c r="J7" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="K7" s="31">
-        <f>hand_players!G7-hand_actions!I7</f>
+      <c r="J7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" s="30">
+        <f>'.hand_players'!G7-'.hand_actions'!I7</f>
         <v>1499500</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="F8" s="24">
-        <f t="shared" ref="F8:F19" si="0">F7+1</f>
+        <f t="shared" ref="F8:F19" si="1">F7+1</f>
         <v>3</v>
       </c>
       <c r="G8" s="24">
-        <f>G7+I7</f>
+        <f t="shared" si="0"/>
         <v>1300</v>
       </c>
       <c r="H8" s="24" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="I8" s="24">
         <v>500</v>
@@ -2391,37 +2859,37 @@
       <c r="J8" s="24" t="b">
         <v>0</v>
       </c>
-      <c r="K8" s="32">
-        <f>hand_players!G8-hand_actions!I8</f>
+      <c r="K8" s="31">
+        <f>'.hand_players'!G8-'.hand_actions'!I8</f>
         <v>799500</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="F9" s="21">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G9" s="21">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G9" s="21">
-        <f>G8+I8</f>
         <v>1800</v>
       </c>
       <c r="H9" s="21" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="I9" s="21">
         <v>0</v>
@@ -2436,68 +2904,68 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="B10" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="C10" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="D10" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="E10" s="33" t="s">
-        <v>92</v>
-      </c>
-      <c r="F10" s="30">
+        <v>72</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="G10" s="2">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="G10" s="30">
-        <f>G9+I9</f>
         <v>1800</v>
       </c>
-      <c r="H10" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="I10" s="30">
-        <v>0</v>
-      </c>
-      <c r="J10" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="K10" s="31">
+      <c r="H10" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K10" s="30">
         <f>K7-I10</f>
         <v>1499500</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="E11" s="27" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="F11" s="24">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="G11" s="24">
-        <f>G10+I10</f>
         <v>1800</v>
       </c>
       <c r="H11" s="24" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="I11" s="24">
         <v>0</v>
@@ -2505,37 +2973,37 @@
       <c r="J11" s="24" t="b">
         <v>0</v>
       </c>
-      <c r="K11" s="32">
+      <c r="K11" s="31">
         <f>K8-I11</f>
         <v>799500</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="F12" s="21">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="G12" s="21">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="G12" s="21">
-        <f>G11+I11</f>
         <v>1800</v>
       </c>
       <c r="H12" s="21" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="I12" s="21">
         <v>0</v>
@@ -2550,145 +3018,145 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="B13" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="C13" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="D13" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="E13" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="F13" s="30">
+        <v>72</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F13" s="2">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="G13" s="2">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="G13" s="30">
-        <f>G12+I12</f>
         <v>1800</v>
       </c>
-      <c r="H13" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="I13" s="30">
-        <v>0</v>
-      </c>
-      <c r="J13" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="K13" s="31">
+      <c r="H13" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0</v>
+      </c>
+      <c r="J13" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" s="30">
         <f>K10</f>
         <v>1499500</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="B14" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="C14" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="D14" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="E14" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="F14" s="30">
+        <v>72</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F14" s="2">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G14" s="2">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="G14" s="30">
-        <f>G13+I13</f>
         <v>1800</v>
       </c>
-      <c r="H14" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="I14" s="30">
+      <c r="H14" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I14" s="2">
         <v>1200</v>
       </c>
-      <c r="J14" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="K14" s="31">
+      <c r="J14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" s="30">
         <f>K11-I14</f>
         <v>798300</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="B15" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="C15" s="30" t="s">
-        <v>122</v>
-      </c>
-      <c r="D15" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="F15" s="30">
+        <v>72</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F15" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G15" s="2">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="G15" s="30">
-        <f>G14+I14</f>
         <v>3000</v>
       </c>
-      <c r="H15" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="I15" s="30">
+      <c r="H15" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I15" s="2">
         <f>I14</f>
         <v>1200</v>
       </c>
-      <c r="J15" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="K15" s="31">
+      <c r="J15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" s="30">
         <f>K12-I15</f>
         <v>998300</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D16" s="27" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="F16" s="24">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="G16" s="24">
         <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="G16" s="24">
-        <f>G15+I15</f>
         <v>4200</v>
       </c>
       <c r="H16" s="24" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="I16" s="24">
         <v>0</v>
@@ -2696,37 +3164,37 @@
       <c r="J16" s="24" t="b">
         <v>0</v>
       </c>
-      <c r="K16" s="32">
+      <c r="K16" s="31">
         <f>K13</f>
         <v>1499500</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="F17" s="21">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="G17" s="21">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="G17" s="21">
-        <f>G16+I16</f>
         <v>4200</v>
       </c>
       <c r="H17" s="21" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="I17" s="21">
         <v>0</v>
@@ -2741,106 +3209,106 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="B18" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="C18" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="D18" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="E18" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="F18" s="30">
+        <v>72</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="G18" s="2">
         <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="G18" s="30">
-        <f>G17+I17</f>
         <v>4200</v>
       </c>
-      <c r="H18" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="I18" s="30">
+      <c r="H18" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I18" s="2">
         <v>1200</v>
       </c>
-      <c r="J18" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="K18" s="31">
+      <c r="J18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K18" s="30">
         <f>K14-I18</f>
         <v>797100</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="B19" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="C19" s="30" t="s">
-        <v>122</v>
-      </c>
-      <c r="D19" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="E19" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="F19" s="30">
+        <v>72</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F19" s="2">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="G19" s="2">
         <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="G19" s="30">
-        <f>G18+I18</f>
         <v>5400</v>
       </c>
-      <c r="H19" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="I19" s="30">
+      <c r="H19" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I19" s="2">
         <f>K17</f>
         <v>998300</v>
       </c>
-      <c r="J19" s="30" t="b">
+      <c r="J19" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="K19" s="31">
+      <c r="K19" s="30">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="E20" s="24" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="F20" s="24">
-        <f t="shared" ref="F20" si="1">F19+1</f>
+        <f t="shared" ref="F20" si="2">F19+1</f>
         <v>15</v>
       </c>
       <c r="G20" s="24">
-        <f>G19+I19</f>
+        <f t="shared" si="0"/>
         <v>1003700</v>
       </c>
       <c r="H20" s="24" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="I20" s="24">
         <v>0</v>
@@ -2848,7 +3316,7 @@
       <c r="J20" s="24" t="b">
         <v>0</v>
       </c>
-      <c r="K20" s="32">
+      <c r="K20" s="31">
         <f>K18</f>
         <v>797100</v>
       </c>
@@ -2882,390 +3350,212 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DE0DFDF-D9E5-8B47-B89F-323429675129}">
-  <dimension ref="A1:I11"/>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E595855-FCC9-CD4F-A83B-9F0E43C081E7}">
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="42.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="B1" s="18" t="s">
+    <row r="1" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="B8" s="2">
+        <v>100</v>
+      </c>
+      <c r="C8" s="2">
+        <v>200</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="I1" s="17" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="B2" s="19">
-        <v>1</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="B3" s="19">
-        <v>2</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="B4" s="19">
-        <v>3</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="10"/>
-      <c r="B5" s="19">
-        <v>4</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="10"/>
-      <c r="B6" s="19">
-        <v>5</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="10"/>
-      <c r="B7" s="19">
-        <v>6</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="10"/>
-      <c r="B8" s="19">
-        <v>7</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="10"/>
-      <c r="B9" s="19">
-        <v>8</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="10"/>
-      <c r="B10" s="19">
-        <v>9</v>
-      </c>
-      <c r="C10" s="10" t="s">
+      <c r="E8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="10"/>
-      <c r="B11" s="19">
-        <v>10</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
+      <c r="B9" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="9"/>
+      <c r="C12" s="9"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="15"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D39D9E3-0EB2-BA4D-9DA7-B5A172AB8C82}">
-  <dimension ref="A1:E17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="13.1640625" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>73</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C16" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{3AFABB3D-38C0-CA4B-96C5-C68C5E1F75DE}">
+      <formula1>DataLayouts</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:F5" xr:uid="{2B43068A-F86C-2F43-9DA6-BD346589A1EE}">
+      <formula1>TableDataTypes</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
support _null_ as a valid cell entry
</commit_message>
<xml_diff>
--- a/packages/pg/tests/test-pg-data-loading.xlsx
+++ b/packages/pg/tests/test-pg-data-loading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Documents/sentosa/code/stcland/packages/pg/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA79550F-BB85-DE4D-8980-6EAF24505A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD5E6B6-E954-8949-B885-6F421B52A946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13480" yWindow="6520" windowWidth="34560" windowHeight="19440" activeTab="3" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
   </bookViews>
@@ -591,7 +591,7 @@
     <t>Winter</t>
   </si>
   <si>
-    <t>null</t>
+    <t>_skip_</t>
   </si>
 </sst>
 </file>
@@ -1895,7 +1895,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
complete postgres data parser
</commit_message>
<xml_diff>
--- a/packages/pg/tests/test-pg-data-loading.xlsx
+++ b/packages/pg/tests/test-pg-data-loading.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Documents/sentosa/code/stcland/packages/pg/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28BB919C-EB77-E64E-8A4F-6995AFE24BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3B1F60-5841-E247-89B4-DC92323E653B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4040" yWindow="3440" windowWidth="28540" windowHeight="20760" activeTab="5" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
+    <workbookView xWindow="12940" yWindow="760" windowWidth="19680" windowHeight="19980" firstSheet="3" activeTab="7" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
   </bookViews>
   <sheets>
     <sheet name="organizations" sheetId="9" r:id="rId1"/>
@@ -19,20 +19,24 @@
     <sheet name="players" sheetId="11" r:id="rId4"/>
     <sheet name="hand_groups" sheetId="20" r:id="rId5"/>
     <sheet name="hands" sheetId="1" r:id="rId6"/>
-    <sheet name="hands_players" sheetId="15" r:id="rId7"/>
-    <sheet name="hand_actions" sheetId="16" r:id="rId8"/>
-    <sheet name=".cash_stakes" sheetId="13" r:id="rId9"/>
-    <sheet name=".tables" sheetId="12" r:id="rId10"/>
-    <sheet name=".enums" sheetId="17" r:id="rId11"/>
-    <sheet name=".lists" sheetId="7" r:id="rId12"/>
+    <sheet name="forced_bets" sheetId="22" r:id="rId7"/>
+    <sheet name="hands_players" sheetId="15" r:id="rId8"/>
+    <sheet name="hand_actions" sheetId="16" r:id="rId9"/>
+    <sheet name=".cash_stakes" sheetId="13" r:id="rId10"/>
+    <sheet name=".tables" sheetId="12" r:id="rId11"/>
+    <sheet name=".enums" sheetId="17" r:id="rId12"/>
+    <sheet name=".lists" sheetId="7" r:id="rId13"/>
   </sheets>
   <definedNames>
-    <definedName name="_Action">'.enums'!$I$2:$I$6</definedName>
+    <definedName name="_Action">'.enums'!$I$2:$I$7</definedName>
     <definedName name="_Actions">'.enums'!$I$2:$I$6</definedName>
+    <definedName name="_Archetype">'.enums'!$C$17:$C$23</definedName>
+    <definedName name="_Currencies">'.enums'!$B$17:$B$26</definedName>
+    <definedName name="_ForcedBetTypes">'.enums'!$A$17:$A$20</definedName>
     <definedName name="_GameFormats">'.enums'!$E$2:$E$3</definedName>
     <definedName name="_GameTypes">'.enums'!$D$2:$D$3</definedName>
     <definedName name="_HandGroupTypes">'.enums'!$J$2:$J$4</definedName>
-    <definedName name="_HandResults">'.enums'!$K$2:$K$4</definedName>
+    <definedName name="_HandResults">'.enums'!$K$2:$K$5</definedName>
     <definedName name="_Position">'.enums'!$C$2:$C$11</definedName>
     <definedName name="_Positions">'.enums'!$C$2:$C$11</definedName>
     <definedName name="_Roles">'.enums'!$A$2:$A$4</definedName>
@@ -40,7 +44,6 @@
     <definedName name="_Street">'.enums'!$H$2:$H$5</definedName>
     <definedName name="_Streets">'.enums'!$H$2:$H$5</definedName>
     <definedName name="_VenueTypes">'.enums'!$F$2:$F$3</definedName>
-    <definedName name="Currencies">'.enums'!$G$2:$G$4</definedName>
     <definedName name="DataLayouts">'.lists'!$E$2:$E$4</definedName>
     <definedName name="ListDataTypes">'.lists'!$C$2:$C$17</definedName>
     <definedName name="TableDataTypes">'.lists'!$A$2:$A$10</definedName>
@@ -64,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="222">
   <si>
     <t>number</t>
   </si>
@@ -147,469 +150,589 @@
     <t>user_id</t>
   </si>
   <si>
+    <t>stevo</t>
+  </si>
+  <si>
+    <t>steve@sentosatech.com</t>
+  </si>
+  <si>
+    <t>gabe</t>
+  </si>
+  <si>
+    <t>gabe@sentosatech.com</t>
+  </si>
+  <si>
+    <t>small_blind</t>
+  </si>
+  <si>
+    <t>big_blind</t>
+  </si>
+  <si>
+    <t>$1/$3</t>
+  </si>
+  <si>
+    <t>$2/$5</t>
+  </si>
+  <si>
+    <t>NL25</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>NL50</t>
+  </si>
+  <si>
+    <t>First Table Ever</t>
+  </si>
+  <si>
+    <t>game_type</t>
+  </si>
+  <si>
+    <t>NLHE</t>
+  </si>
+  <si>
+    <t>stakes</t>
+  </si>
+  <si>
+    <t>BTN</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>uuid:ref</t>
+  </si>
+  <si>
+    <t>uuid:link</t>
+  </si>
+  <si>
+    <t>1_3:_auto_</t>
+  </si>
+  <si>
+    <t>2_5:_auto_</t>
+  </si>
+  <si>
+    <t>nl25:_auto_</t>
+  </si>
+  <si>
+    <t>nl50:_auto_</t>
+  </si>
+  <si>
+    <t>hand1:_auto_</t>
+  </si>
+  <si>
+    <t>hands.hand1</t>
+  </si>
+  <si>
+    <t>_auto_</t>
+  </si>
+  <si>
+    <t>ADMIN</t>
+  </si>
+  <si>
+    <t>CASH</t>
+  </si>
+  <si>
+    <t>ONLINE</t>
+  </si>
+  <si>
+    <t>PRE_FLOP</t>
+  </si>
+  <si>
+    <t>CHECK</t>
+  </si>
+  <si>
+    <t>USER</t>
+  </si>
+  <si>
+    <t>SB</t>
+  </si>
+  <si>
+    <t>PLO</t>
+  </si>
+  <si>
+    <t>TOURNAMENT</t>
+  </si>
+  <si>
+    <t>LIVE</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>FLOP</t>
+  </si>
+  <si>
+    <t>CALL</t>
+  </si>
+  <si>
+    <t>COACH</t>
+  </si>
+  <si>
+    <t>UTG</t>
+  </si>
+  <si>
+    <t>GBP</t>
+  </si>
+  <si>
+    <t>TURN</t>
+  </si>
+  <si>
+    <t>BET</t>
+  </si>
+  <si>
+    <t>UTG+1</t>
+  </si>
+  <si>
+    <t>RIVER</t>
+  </si>
+  <si>
+    <t>RAISE</t>
+  </si>
+  <si>
+    <t>UTG+2</t>
+  </si>
+  <si>
+    <t>FOLD</t>
+  </si>
+  <si>
+    <t>UTG+3</t>
+  </si>
+  <si>
+    <t>LJ</t>
+  </si>
+  <si>
+    <t>HJ</t>
+  </si>
+  <si>
+    <t>num_seats</t>
+  </si>
+  <si>
+    <t>h1_p_haxton:_auto_</t>
+  </si>
+  <si>
+    <t>h1_p_foxen:_auto_</t>
+  </si>
+  <si>
+    <t>h1_p_winter:_auto_</t>
+  </si>
+  <si>
+    <t>p_steve:_auto_</t>
+  </si>
+  <si>
+    <t>p_gabe:_auto_</t>
+  </si>
+  <si>
+    <t>p_haxton:_auto_</t>
+  </si>
+  <si>
+    <t>p_foxen:_auto_</t>
+  </si>
+  <si>
+    <t>players.p_haxton</t>
+  </si>
+  <si>
+    <t>players.p_foxen</t>
+  </si>
+  <si>
+    <t>players.p_winter</t>
+  </si>
+  <si>
+    <t>_Roles</t>
+  </si>
+  <si>
+    <t>_SeatNums</t>
+  </si>
+  <si>
+    <t>_Positions</t>
+  </si>
+  <si>
+    <t>_GameTypes</t>
+  </si>
+  <si>
+    <t>_GameFormats</t>
+  </si>
+  <si>
+    <t>_VenueTypes</t>
+  </si>
+  <si>
+    <t>_Currencies</t>
+  </si>
+  <si>
+    <t>_Streets</t>
+  </si>
+  <si>
+    <t>_Actions</t>
+  </si>
+  <si>
+    <t>100_200:_auto_</t>
+  </si>
+  <si>
+    <t>$100/$200</t>
+  </si>
+  <si>
+    <t>position</t>
+  </si>
+  <si>
+    <t>is_all_in</t>
+  </si>
+  <si>
+    <t>u_steve:_auto_</t>
+  </si>
+  <si>
+    <t>u_gabe:_auto_</t>
+  </si>
+  <si>
+    <t>users.u_steve</t>
+  </si>
+  <si>
+    <t>users.u_gabe</t>
+  </si>
+  <si>
+    <t>p_winter:_auto_</t>
+  </si>
+  <si>
+    <t>table1:_auto_</t>
+  </si>
+  <si>
+    <t>cash_stakes.100_200</t>
+  </si>
+  <si>
+    <t>hand_id</t>
+  </si>
+  <si>
+    <t>hand_player_id</t>
+  </si>
+  <si>
+    <t>street</t>
+  </si>
+  <si>
+    <t>action_sequence</t>
+  </si>
+  <si>
+    <t>action</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>is_custom</t>
+  </si>
+  <si>
+    <t>org_tbs:_auto_</t>
+  </si>
+  <si>
+    <t>org_cpg:_auto_</t>
+  </si>
+  <si>
+    <t>Triple Barrel Software</t>
+  </si>
+  <si>
+    <t>u_brad:_auto_</t>
+  </si>
+  <si>
+    <t>brad@chasingpokergreatness.com</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>Steve</t>
+  </si>
+  <si>
+    <t>Saunders</t>
+  </si>
+  <si>
+    <t>Gabe</t>
+  </si>
+  <si>
+    <t>Alex-something</t>
+  </si>
+  <si>
+    <t>Brad</t>
+  </si>
+  <si>
+    <t>Wilson</t>
+  </si>
+  <si>
+    <t>organization_id</t>
+  </si>
+  <si>
+    <t>users.u_brad</t>
+  </si>
+  <si>
+    <t>organizations.org_tbs</t>
+  </si>
+  <si>
+    <t>organizations.org_cpg</t>
+  </si>
+  <si>
+    <t>p_brad:_auto_</t>
+  </si>
+  <si>
+    <t>Isaac</t>
+  </si>
+  <si>
+    <t>Haxton</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Foxen</t>
+  </si>
+  <si>
+    <t>Sean</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>_null_</t>
+  </si>
+  <si>
+    <t>h_group1:_auto_</t>
+  </si>
+  <si>
+    <t>group_type</t>
+  </si>
+  <si>
+    <t>_HandGroupTypes</t>
+  </si>
+  <si>
+    <t>SESSION</t>
+  </si>
+  <si>
+    <t>FEATURED_PLAYER</t>
+  </si>
+  <si>
+    <t>HOMEWORK</t>
+  </si>
+  <si>
+    <t>agent_id</t>
+  </si>
+  <si>
+    <t>hand_groups.h_group1</t>
+  </si>
+  <si>
+    <t>hand_group_id</t>
+  </si>
+  <si>
+    <t>hand_number</t>
+  </si>
+  <si>
+    <t>num_players_seated</t>
+  </si>
+  <si>
+    <t>result</t>
+  </si>
+  <si>
+    <t>_HandResults</t>
+  </si>
+  <si>
+    <t>WON</t>
+  </si>
+  <si>
+    <t>LOST</t>
+  </si>
+  <si>
+    <t>SPLIT</t>
+  </si>
+  <si>
+    <t>player_id</t>
+  </si>
+  <si>
+    <t>hole_cards</t>
+  </si>
+  <si>
+    <t>starting_stack</t>
+  </si>
+  <si>
+    <t>ending_stack</t>
+  </si>
+  <si>
+    <t>[ "Jd", "Jh" ]</t>
+  </si>
+  <si>
+    <t>Chasing Poker Greatness</t>
+  </si>
+  <si>
+    <t>[ "Ac", "Kd" ]</t>
+  </si>
+  <si>
+    <t>[ "9s", "Ts" ]</t>
+  </si>
+  <si>
+    <t>hands_players.h1_p_haxton</t>
+  </si>
+  <si>
+    <t>hands_players.h1_p_foxen</t>
+  </si>
+  <si>
+    <t>hands_players.h1_p_winter</t>
+  </si>
+  <si>
+    <t>community_cards</t>
+  </si>
+  <si>
+    <t>["8s", "Qh", "Qd", "Kc", "2s"]</t>
+  </si>
+  <si>
+    <t>bradley</t>
+  </si>
+  <si>
+    <t>TO_ACT</t>
+  </si>
+  <si>
+    <t>hero_position</t>
+  </si>
+  <si>
+    <t>_ForcedBetTypes</t>
+  </si>
+  <si>
+    <t>STRADDLE</t>
+  </si>
+  <si>
+    <t>BIG_BLIND</t>
+  </si>
+  <si>
+    <t>SMALL_BLIND</t>
+  </si>
+  <si>
+    <t>ANTE</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  USD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  EUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  GBP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  JPY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  CNY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  INR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  AUD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  CAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  CHF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  NZD</t>
+  </si>
+  <si>
+    <t>bet_number</t>
+  </si>
+  <si>
+    <t>gcrush</t>
+  </si>
+  <si>
+    <t>badbrad</t>
+  </si>
+  <si>
+    <t>hax</t>
+  </si>
+  <si>
+    <t>fox</t>
+  </si>
+  <si>
+    <t>snow</t>
+  </si>
+  <si>
+    <t>archetype</t>
+  </si>
+  <si>
+    <t>_Archetype</t>
+  </si>
+  <si>
+    <t>CRUSHER</t>
+  </si>
+  <si>
+    <t>REGULAR</t>
+  </si>
+  <si>
+    <t>CALLING_STATION</t>
+  </si>
+  <si>
+    <t>OLD_MAN_COFFEE</t>
+  </si>
+  <si>
+    <t>NIT</t>
+  </si>
+  <si>
+    <t>MANIAC</t>
+  </si>
+  <si>
+    <t>FISH</t>
+  </si>
+  <si>
     <t>nickname</t>
   </si>
   <si>
-    <t>stevo</t>
-  </si>
-  <si>
-    <t>steve@sentosatech.com</t>
-  </si>
-  <si>
-    <t>gabe</t>
-  </si>
-  <si>
-    <t>gabe@sentosatech.com</t>
-  </si>
-  <si>
-    <t>Stevo</t>
-  </si>
-  <si>
-    <t>Gabe the Crusher</t>
-  </si>
-  <si>
-    <t>AlexF</t>
-  </si>
-  <si>
-    <t>IkeH</t>
-  </si>
-  <si>
-    <t>SeanW</t>
-  </si>
-  <si>
-    <t>small_blind</t>
-  </si>
-  <si>
-    <t>big_blind</t>
-  </si>
-  <si>
-    <t>$1/$3</t>
-  </si>
-  <si>
-    <t>$2/$5</t>
-  </si>
-  <si>
-    <t>NL25</t>
-  </si>
-  <si>
-    <t>currency</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>NL50</t>
-  </si>
-  <si>
-    <t>First Table Ever</t>
-  </si>
-  <si>
-    <t>game_type</t>
-  </si>
-  <si>
-    <t>NLHE</t>
-  </si>
-  <si>
-    <t>stakes</t>
-  </si>
-  <si>
-    <t>BTN</t>
-  </si>
-  <si>
-    <t>BB</t>
-  </si>
-  <si>
-    <t>CO</t>
-  </si>
-  <si>
-    <t>uuid:ref</t>
-  </si>
-  <si>
-    <t>uuid:link</t>
-  </si>
-  <si>
-    <t>1_3:_auto_</t>
-  </si>
-  <si>
-    <t>2_5:_auto_</t>
-  </si>
-  <si>
-    <t>nl25:_auto_</t>
-  </si>
-  <si>
-    <t>nl50:_auto_</t>
-  </si>
-  <si>
-    <t>hand1:_auto_</t>
-  </si>
-  <si>
-    <t>hands.hand1</t>
-  </si>
-  <si>
-    <t>_auto_</t>
-  </si>
-  <si>
-    <t>ADMIN</t>
-  </si>
-  <si>
-    <t>CASH</t>
-  </si>
-  <si>
-    <t>ONLINE</t>
-  </si>
-  <si>
-    <t>PRE_FLOP</t>
-  </si>
-  <si>
-    <t>CHECK</t>
-  </si>
-  <si>
-    <t>USER</t>
-  </si>
-  <si>
-    <t>SB</t>
-  </si>
-  <si>
-    <t>PLO</t>
-  </si>
-  <si>
-    <t>TOURNAMENT</t>
-  </si>
-  <si>
-    <t>LIVE</t>
-  </si>
-  <si>
-    <t>EUR</t>
-  </si>
-  <si>
-    <t>FLOP</t>
-  </si>
-  <si>
-    <t>CALL</t>
-  </si>
-  <si>
-    <t>COACH</t>
-  </si>
-  <si>
-    <t>UTG</t>
-  </si>
-  <si>
-    <t>GBP</t>
-  </si>
-  <si>
-    <t>TURN</t>
-  </si>
-  <si>
-    <t>BET</t>
-  </si>
-  <si>
-    <t>UTG+1</t>
-  </si>
-  <si>
-    <t>RIVER</t>
-  </si>
-  <si>
-    <t>RAISE</t>
-  </si>
-  <si>
-    <t>UTG+2</t>
-  </si>
-  <si>
-    <t>FOLD</t>
-  </si>
-  <si>
-    <t>UTG+3</t>
-  </si>
-  <si>
-    <t>LJ</t>
-  </si>
-  <si>
-    <t>HJ</t>
-  </si>
-  <si>
-    <t>num_seats</t>
-  </si>
-  <si>
-    <t>h1_p_haxton:_auto_</t>
-  </si>
-  <si>
-    <t>h1_p_foxen:_auto_</t>
-  </si>
-  <si>
-    <t>h1_p_winter:_auto_</t>
-  </si>
-  <si>
-    <t>p_steve:_auto_</t>
-  </si>
-  <si>
-    <t>p_gabe:_auto_</t>
-  </si>
-  <si>
-    <t>p_haxton:_auto_</t>
-  </si>
-  <si>
-    <t>p_foxen:_auto_</t>
-  </si>
-  <si>
-    <t>players.p_haxton</t>
-  </si>
-  <si>
-    <t>players.p_foxen</t>
-  </si>
-  <si>
-    <t>players.p_winter</t>
-  </si>
-  <si>
-    <t>_Roles</t>
-  </si>
-  <si>
-    <t>_SeatNums</t>
-  </si>
-  <si>
-    <t>_Positions</t>
-  </si>
-  <si>
-    <t>_GameTypes</t>
-  </si>
-  <si>
-    <t>_GameFormats</t>
-  </si>
-  <si>
-    <t>_VenueTypes</t>
-  </si>
-  <si>
-    <t>_Currencies</t>
-  </si>
-  <si>
-    <t>_Streets</t>
-  </si>
-  <si>
-    <t>_Actions</t>
-  </si>
-  <si>
-    <t>100_200:_auto_</t>
-  </si>
-  <si>
-    <t>$100/$200</t>
-  </si>
-  <si>
-    <t>position</t>
-  </si>
-  <si>
     <t>dealer_seat_num</t>
   </si>
   <si>
-    <t>is_all_in</t>
-  </si>
-  <si>
-    <t>u_steve:_auto_</t>
-  </si>
-  <si>
-    <t>u_gabe:_auto_</t>
-  </si>
-  <si>
-    <t>users.u_steve</t>
-  </si>
-  <si>
-    <t>users.u_gabe</t>
-  </si>
-  <si>
-    <t>p_winter:_auto_</t>
-  </si>
-  <si>
-    <t>table1:_auto_</t>
-  </si>
-  <si>
-    <t>cash_stakes.100_200</t>
-  </si>
-  <si>
-    <t>hand_id</t>
-  </si>
-  <si>
-    <t>hand_player_id</t>
-  </si>
-  <si>
-    <t>street</t>
-  </si>
-  <si>
-    <t>action_sequence</t>
-  </si>
-  <si>
-    <t>action</t>
-  </si>
-  <si>
-    <t>amount</t>
-  </si>
-  <si>
-    <t>is_custom</t>
-  </si>
-  <si>
-    <t>org_tbs:_auto_</t>
-  </si>
-  <si>
-    <t>org_cpg:_auto_</t>
-  </si>
-  <si>
-    <t>Triple Barrel Software</t>
-  </si>
-  <si>
-    <t>u_brad:_auto_</t>
-  </si>
-  <si>
-    <t>brad@chasingpokergreatness.com</t>
-  </si>
-  <si>
-    <t>bradly</t>
-  </si>
-  <si>
-    <t>first_name</t>
-  </si>
-  <si>
-    <t>last_name</t>
-  </si>
-  <si>
-    <t>Steve</t>
-  </si>
-  <si>
-    <t>Saunders</t>
-  </si>
-  <si>
-    <t>Gabe</t>
-  </si>
-  <si>
-    <t>Alex-something</t>
-  </si>
-  <si>
-    <t>Brad</t>
-  </si>
-  <si>
-    <t>Wilson</t>
-  </si>
-  <si>
-    <t>organization_id</t>
-  </si>
-  <si>
-    <t>users.u_brad</t>
-  </si>
-  <si>
-    <t>organizations.org_tbs</t>
-  </si>
-  <si>
-    <t>organizations.org_cpg</t>
-  </si>
-  <si>
-    <t>p_brad:_auto_</t>
-  </si>
-  <si>
-    <t>Bad Brad</t>
-  </si>
-  <si>
-    <t>Isaac</t>
-  </si>
-  <si>
-    <t>Haxton</t>
-  </si>
-  <si>
-    <t>Alex</t>
-  </si>
-  <si>
-    <t>Foxen</t>
-  </si>
-  <si>
-    <t>Sean</t>
-  </si>
-  <si>
-    <t>Winter</t>
-  </si>
-  <si>
-    <t>_null_</t>
-  </si>
-  <si>
-    <t>h_group1:_auto_</t>
-  </si>
-  <si>
-    <t>group_type</t>
-  </si>
-  <si>
-    <t>_HandGroupTypes</t>
-  </si>
-  <si>
-    <t>SESSION</t>
-  </si>
-  <si>
-    <t>FEATURED_PLAYER</t>
-  </si>
-  <si>
-    <t>HOMEWORK</t>
-  </si>
-  <si>
-    <t>agent_id</t>
-  </si>
-  <si>
-    <t>hand_groups.h_group1</t>
-  </si>
-  <si>
-    <t>hand_group_id</t>
-  </si>
-  <si>
-    <t>hand_number</t>
-  </si>
-  <si>
-    <t>num_players_seated</t>
-  </si>
-  <si>
-    <t>result</t>
-  </si>
-  <si>
-    <t>_HandResults</t>
-  </si>
-  <si>
-    <t>WON</t>
-  </si>
-  <si>
-    <t>LOST</t>
-  </si>
-  <si>
-    <t>SPLIT</t>
-  </si>
-  <si>
-    <t>player_id</t>
-  </si>
-  <si>
-    <t>hole_cards</t>
-  </si>
-  <si>
-    <t>starting_stack</t>
-  </si>
-  <si>
-    <t>ending_stack</t>
-  </si>
-  <si>
-    <t>[ "Jd", "Jh" ]</t>
-  </si>
-  <si>
-    <t>Chasing Poker Greatness</t>
-  </si>
-  <si>
-    <t>[ "Ac", "Kd" ]</t>
-  </si>
-  <si>
-    <t>[ "9s", "Ts" ]</t>
-  </si>
-  <si>
-    <t>hands_players.h1_p_haxton</t>
-  </si>
-  <si>
-    <t>hands_players.h1_p_foxen</t>
-  </si>
-  <si>
-    <t>hands_players.h1_p_winter</t>
-  </si>
-  <si>
-    <t>community_cards</t>
-  </si>
-  <si>
-    <t>["8s", "Qh", "Qd", "Kc", "2s"]</t>
+    <t>IN_PROGRESS</t>
+  </si>
+  <si>
+    <t>hand2:_auto_</t>
+  </si>
+  <si>
+    <t>["As", "Qs", "5d", "Kc"]</t>
+  </si>
+  <si>
+    <t>[ "Ad", "5s" ]</t>
+  </si>
+  <si>
+    <t>[ "Qd", "5s" ]</t>
+  </si>
+  <si>
+    <t>[ "Kd", "Ks" ]</t>
+  </si>
+  <si>
+    <t>hands.hand2</t>
+  </si>
+  <si>
+    <t>h2_p_haxton:_auto_</t>
+  </si>
+  <si>
+    <t>h2_p_foxen:_auto_</t>
+  </si>
+  <si>
+    <t>h2_p_winter:_auto_</t>
+  </si>
+  <si>
+    <t>hands_players.h2_p_haxton</t>
+  </si>
+  <si>
+    <t>hands_players.h2_p_foxen</t>
+  </si>
+  <si>
+    <t>hands_players.h2_p_winter</t>
   </si>
 </sst>
 </file>
@@ -794,7 +917,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -864,10 +987,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1184,10 +1328,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0992D42-8EDD-1644-B63D-73C3203972BD}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1224,7 +1369,7 @@
     </row>
     <row r="5" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>1</v>
@@ -1232,18 +1377,18 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1271,10 +1416,223 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E595855-FCC9-CD4F-A83B-9F0E43C081E7}">
+  <sheetPr codeName="Sheet9"/>
+  <dimension ref="A1:F16"/>
+  <sheetViews>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="42.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="2">
+        <v>100</v>
+      </c>
+      <c r="C8" s="2">
+        <v>200</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="8"/>
+      <c r="C12" s="8"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="13"/>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{3AFABB3D-38C0-CA4B-96C5-C68C5E1F75DE}">
+      <formula1>DataLayouts</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:F5" xr:uid="{2B43068A-F86C-2F43-9DA6-BD346589A1EE}">
+      <formula1>TableDataTypes</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE849852-9B8D-D646-983A-87B67FBBE846}">
+  <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -1313,18 +1671,18 @@
         <v>8</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>1</v>
@@ -1333,7 +1691,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>0</v>
@@ -1341,16 +1699,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="E6" s="2">
         <v>6</v>
@@ -1404,16 +1762,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DE0DFDF-D9E5-8B47-B89F-323429675129}">
-  <dimension ref="A1:K11"/>
+  <sheetPr codeName="Sheet11"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" customWidth="1"/>
@@ -1423,136 +1785,136 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G1" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="H1" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="I1" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="D1" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>106</v>
-      </c>
       <c r="J1" s="15" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B2" s="17">
         <v>1</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B3" s="17">
         <v>2</v>
       </c>
       <c r="C3" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>73</v>
-      </c>
       <c r="J3" s="9" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B4" s="17">
         <v>3</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -1561,17 +1923,20 @@
         <v>4</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="H5" s="9" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>81</v>
+        <v>75</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -1580,7 +1945,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -1588,7 +1953,7 @@
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -1597,14 +1962,16 @@
         <v>6</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
+      <c r="I7" s="9" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="9"/>
@@ -1612,7 +1979,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
@@ -1627,7 +1994,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
@@ -1642,7 +2009,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
@@ -1657,7 +2024,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
@@ -1666,13 +2033,109 @@
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
     </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>179</v>
+      </c>
+      <c r="B17" t="s">
+        <v>182</v>
+      </c>
+      <c r="C17" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>178</v>
+      </c>
+      <c r="B18" t="s">
+        <v>183</v>
+      </c>
+      <c r="C18" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>177</v>
+      </c>
+      <c r="B19" t="s">
+        <v>184</v>
+      </c>
+      <c r="C19" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>180</v>
+      </c>
+      <c r="B20" t="s">
+        <v>185</v>
+      </c>
+      <c r="C20" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>186</v>
+      </c>
+      <c r="C21" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>187</v>
+      </c>
+      <c r="C22" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>188</v>
+      </c>
+      <c r="C23" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>191</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D39D9E3-0EB2-BA4D-9DA7-B5A172AB8C82}">
+  <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -1764,7 +2227,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
         <v>13</v>
@@ -1772,7 +2235,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
@@ -1805,12 +2268,12 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1821,10 +2284,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BF7FE8D-D3D6-0341-A57E-3BE902F737F0}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:E8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1865,15 +2329,15 @@
         <v>25</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>1</v>
@@ -1890,53 +2354,53 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>29</v>
-      </c>
       <c r="D6" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="E6" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>31</v>
-      </c>
       <c r="D7" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="E7" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1950,7 +2414,7 @@
       <c r="A16" s="13"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations disablePrompts="1" count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:E5" xr:uid="{A5363200-5E32-0A4E-98B4-61E0F10BE994}">
       <formula1>TableDataTypes</formula1>
     </dataValidation>
@@ -1968,10 +2432,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EA6A974-E798-9241-8093-8124B9D0B6E3}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A5"/>
+    <sheetView zoomScale="130" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2003,39 +2468,39 @@
         <v>26</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -2049,7 +2514,7 @@
       <c r="A16" s="13"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{1388F5CC-5F3E-6E43-9598-EC3C28E06242}">
       <formula1>DataLayouts</formula1>
     </dataValidation>
@@ -2064,22 +2529,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2263EDC9-A2CB-9C45-8C08-CE3DC9B88E26}">
-  <dimension ref="A1:E17"/>
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="38.6640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="17.1640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="17.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>12</v>
       </c>
@@ -2087,17 +2553,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
@@ -2105,21 +2571,24 @@
         <v>26</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>27</v>
+        <v>124</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+        <v>207</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>1</v>
@@ -2130,138 +2599,160 @@
       <c r="E5" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>32</v>
+        <v>107</v>
+      </c>
+      <c r="C6" t="s">
+        <v>126</v>
       </c>
       <c r="D6" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="E6" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>33</v>
+        <v>108</v>
+      </c>
+      <c r="C7" t="s">
+        <v>128</v>
       </c>
       <c r="D7" t="s">
+        <v>129</v>
+      </c>
+      <c r="E7" t="s">
+        <v>193</v>
+      </c>
+      <c r="F7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>136</v>
       </c>
-      <c r="E7" t="s">
+      <c r="B8" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="F8" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>144</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="D9" t="s">
+        <v>138</v>
+      </c>
+      <c r="E9" t="s">
+        <v>195</v>
+      </c>
+      <c r="F9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D10" t="s">
+        <v>140</v>
+      </c>
+      <c r="E10" t="s">
+        <v>196</v>
+      </c>
+      <c r="F10" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>93</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>152</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="E9" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>94</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>152</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="E10" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>116</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>152</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>150</v>
+      <c r="D11" t="s">
+        <v>142</v>
       </c>
       <c r="E11" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>197</v>
+      </c>
+      <c r="F11" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="8"/>
-      <c r="C13" s="8"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D16" s="3"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C16" s="3"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="13"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{F80FB675-602B-2544-8804-620039F78CFA}">
       <formula1>DataLayouts</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:E5" xr:uid="{227E0E5E-8598-1C4B-A6FF-1AF8F3D32A17}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:F5" xr:uid="{227E0E5E-8598-1C4B-A6FF-1AF8F3D32A17}">
       <formula1>TableDataTypes</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F11" xr:uid="{16EE595A-5A32-DA4B-B61B-4CB7EEFDED5C}">
+      <formula1>_Archetype</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2271,10 +2762,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DCE8850-934F-2941-99F1-09B5725B2027}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2308,32 +2800,32 @@
         <v>23</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -2402,19 +2894,220 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B101DD8F-9A36-0342-BC29-1E3C3A22B2B5}">
-  <dimension ref="A1:F16"/>
+  <sheetPr codeName="Sheet6"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="36.83203125" style="2" customWidth="1"/>
-    <col min="2" max="3" width="20.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="19.1640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" customWidth="1"/>
-    <col min="6" max="6" width="28.1640625" customWidth="1"/>
+    <col min="2" max="4" width="20.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="19.1640625" style="2" customWidth="1"/>
+    <col min="6" max="7" width="16.83203125" customWidth="1"/>
+    <col min="8" max="8" width="28.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="2">
+        <v>8</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>210</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="2">
+        <v>8</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F15" s="2"/>
+      <c r="G15" s="9"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="13"/>
+    </row>
+  </sheetData>
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5" xr:uid="{A7427D63-E072-9D43-B99E-939C11A4ABCC}">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{41DFCB9E-CA3F-8C4F-97D5-E9B20C0F40BC}">
+      <formula1>DataLayouts</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:H5" xr:uid="{FB632601-5BD8-4B42-ACD7-4B96F03BA7D3}">
+      <formula1>TableDataTypes</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G7" xr:uid="{EC385ADA-AF09-E342-B262-A2A697B85FF0}">
+      <formula1>_Positions</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D7" xr:uid="{C87B65F2-5A2B-5E4F-B4E2-886F6E34D600}">
+      <formula1>_Currencies</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F578E2E2-BA2E-944E-88FC-1A0A13492124}">
+  <sheetPr codeName="Sheet13"/>
+  <dimension ref="A1:F16"/>
+  <sheetViews>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="37.83203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2424,7 +3117,6 @@
       <c r="B1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -2441,102 +3133,184 @@
         <v>23</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>161</v>
+        <v>112</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>110</v>
+        <v>192</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>103</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>180</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>3</v>
+        <v>47</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>160</v>
+        <v>53</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
       </c>
-      <c r="D6" s="2">
-        <v>8</v>
-      </c>
-      <c r="E6" s="2">
+      <c r="D6" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="2">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C9" s="2">
         <v>1</v>
       </c>
-      <c r="F6" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="2">
+        <v>50</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E10" s="2"/>
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C11" s="2">
+        <v>3</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" s="2">
+        <v>200</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E15" s="9"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="13"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5" xr:uid="{A7427D63-E072-9D43-B99E-939C11A4ABCC}">
-      <formula1>#REF!</formula1>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:E11" xr:uid="{948AC9DD-CBE4-AC4C-A21B-EC217E47B4ED}">
+      <formula1>_Positions</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{41DFCB9E-CA3F-8C4F-97D5-E9B20C0F40BC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C1" xr:uid="{B5BCF4B5-0AEC-2647-8621-0022F8AB60E0}">
       <formula1>DataLayouts</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:F5" xr:uid="{FB632601-5BD8-4B42-ACD7-4B96F03BA7D3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D11" xr:uid="{66127501-A143-2445-95DD-4C390174FAC9}">
+      <formula1>_ForcedBetTypes</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:F5" xr:uid="{2B32EAD1-20D1-8146-9B8B-623C095B0025}">
       <formula1>TableDataTypes</formula1>
     </dataValidation>
   </dataValidations>
@@ -2545,18 +3319,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D12000C3-1D3F-1248-BA35-71F90F67C3F6}">
-  <dimension ref="A1:H17"/>
+  <sheetPr codeName="Sheet7"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="37.83203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="28.83203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="39" style="2" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
     <col min="5" max="6" width="18.5" customWidth="1"/>
@@ -2587,36 +3362,36 @@
         <v>23</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>1</v>
@@ -2636,22 +3411,22 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E6" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="F6" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="G6" s="2">
         <v>1000000</v>
@@ -2662,22 +3437,22 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E7" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="F7" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="G7" s="2">
         <v>1500000</v>
@@ -2688,22 +3463,22 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E8" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="F8" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="G8" s="2">
         <v>800000</v>
@@ -2712,44 +3487,97 @@
         <v>1800000</v>
       </c>
     </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>216</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" t="s">
+        <v>212</v>
+      </c>
+      <c r="F9" t="s">
+        <v>158</v>
+      </c>
+      <c r="G9" s="2">
+        <v>500000</v>
+      </c>
+      <c r="H9" s="2">
+        <v>495000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" t="s">
+        <v>213</v>
+      </c>
+      <c r="F10" t="s">
+        <v>158</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="H10" s="2">
+        <v>998500</v>
+      </c>
+    </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C11"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="8"/>
-      <c r="C12"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C13"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C15"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="13"/>
-      <c r="C16"/>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C17"/>
+      <c r="A11" t="s">
+        <v>218</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" t="s">
+        <v>214</v>
+      </c>
+      <c r="F11" t="s">
+        <v>157</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1800000</v>
+      </c>
+      <c r="H11" s="2">
+        <v>1806500</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{D02B3419-A22A-A844-A63A-CC8E874B950D}">
       <formula1>DataLayouts</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D8" xr:uid="{4C720365-3E43-5544-90E4-29105A26AADC}">
-      <formula1>_Positions</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:H5" xr:uid="{BF96FBEC-45A9-774A-96D9-AAF7A3181366}">
       <formula1>TableDataTypes</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F8" xr:uid="{8F79ADD0-1123-444F-984F-1B55007344F5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F11" xr:uid="{8F79ADD0-1123-444F-984F-1B55007344F5}">
       <formula1>_HandResults</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D11" xr:uid="{4C720365-3E43-5544-90E4-29105A26AADC}">
+      <formula1>_Positions</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2757,12 +3585,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{490F7804-6FAB-AC46-A3F8-9390691D26BA}">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2776,14 +3605,15 @@
     <col min="8" max="8" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="29"/>
+      <c r="E1"/>
+      <c r="F1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -2800,22 +3630,22 @@
         <v>23</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2823,7 +3653,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>1</v>
@@ -2843,16 +3673,16 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E6" s="19">
         <v>500</v>
@@ -2866,21 +3696,21 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="B7" s="29" t="s">
-        <v>178</v>
-      </c>
-      <c r="C7" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="D7" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="E7" s="29">
+        <v>54</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="2">
         <v>500</v>
       </c>
-      <c r="F7" s="29">
+      <c r="F7" s="2">
         <f>F6+1</f>
         <v>2</v>
       </c>
@@ -2890,16 +3720,16 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E8" s="22">
         <v>500</v>
@@ -2914,16 +3744,16 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E9" s="19">
         <v>0</v>
@@ -2938,21 +3768,21 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" s="29" t="s">
-        <v>177</v>
-      </c>
-      <c r="C10" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="D10" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10" s="29">
-        <v>0</v>
-      </c>
-      <c r="F10" s="29">
+        <v>54</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -2962,16 +3792,16 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E11" s="22">
         <v>0</v>
@@ -2986,16 +3816,16 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E12" s="19">
         <v>0</v>
@@ -3010,21 +3840,21 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="B13" s="29" t="s">
-        <v>177</v>
-      </c>
-      <c r="C13" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="D13" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="E13" s="29">
-        <v>0</v>
-      </c>
-      <c r="F13" s="29">
+        <v>54</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -3034,21 +3864,21 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" s="29" t="s">
-        <v>178</v>
-      </c>
-      <c r="C14" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="D14" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="E14" s="29">
+        <v>54</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="2">
         <v>1200</v>
       </c>
-      <c r="F14" s="29">
+      <c r="F14" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -3058,22 +3888,22 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="B15" s="29" t="s">
-        <v>179</v>
-      </c>
-      <c r="C15" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="D15" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="E15" s="29">
+        <v>54</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="2">
         <f>E14</f>
         <v>1200</v>
       </c>
-      <c r="F15" s="29">
+      <c r="F15" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -3083,16 +3913,16 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="21" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="C16" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" s="22" t="s">
         <v>77</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>83</v>
       </c>
       <c r="E16" s="22">
         <v>0</v>
@@ -3107,16 +3937,16 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="18" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E17" s="19">
         <v>0</v>
@@ -3131,21 +3961,21 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="B18" s="29" t="s">
-        <v>178</v>
-      </c>
-      <c r="C18" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="D18" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="E18" s="29">
+        <v>54</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E18" s="2">
         <v>1200</v>
       </c>
-      <c r="F18" s="29">
+      <c r="F18" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -3155,21 +3985,21 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="B19" s="29" t="s">
-        <v>179</v>
-      </c>
-      <c r="C19" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="D19" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="E19" s="29">
+        <v>54</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" s="2">
         <v>998300</v>
       </c>
-      <c r="F19" s="29">
+      <c r="F19" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -3179,16 +4009,16 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="21" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E20" s="22">
         <v>0</v>
@@ -3201,21 +4031,278 @@
         <v>0</v>
       </c>
     </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="C21" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" s="30">
+        <v>500</v>
+      </c>
+      <c r="F21" s="30">
+        <v>1</v>
+      </c>
+      <c r="G21" s="31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" s="14">
+        <v>500</v>
+      </c>
+      <c r="F22" s="14">
+        <f>F21+1</f>
+        <v>2</v>
+      </c>
+      <c r="G22" s="33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="35" t="s">
+        <v>221</v>
+      </c>
+      <c r="C23" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="E23" s="35">
+        <v>500</v>
+      </c>
+      <c r="F23" s="35">
+        <f t="shared" ref="F23:F31" si="2">F22+1</f>
+        <v>3</v>
+      </c>
+      <c r="G23" s="36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="30" t="s">
+        <v>221</v>
+      </c>
+      <c r="C24" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24" s="14">
+        <v>1000</v>
+      </c>
+      <c r="F24" s="30">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="G24" s="31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="C25" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E25" s="14">
+        <v>1000</v>
+      </c>
+      <c r="F25" s="14">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="G25" s="33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="35" t="s">
+        <v>220</v>
+      </c>
+      <c r="C26" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="D26" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="E26" s="14">
+        <v>1000</v>
+      </c>
+      <c r="F26" s="35">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="G26" s="36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="30" t="s">
+        <v>221</v>
+      </c>
+      <c r="C27" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="E27" s="30">
+        <v>0</v>
+      </c>
+      <c r="F27" s="30">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="G27" s="31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E28" s="14">
+        <v>3500</v>
+      </c>
+      <c r="F28" s="14">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="G28" s="33" t="b">
+        <v>0</v>
+      </c>
+    </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B29"/>
+      <c r="A29" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E29" s="14">
+        <v>0</v>
+      </c>
+      <c r="F29" s="14">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="G29" s="33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E30" s="14">
+        <v>1798500</v>
+      </c>
+      <c r="F30" s="14">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="G30" s="33" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B31"/>
+      <c r="A31" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" s="35" t="s">
+        <v>219</v>
+      </c>
+      <c r="C31" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="D31" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="E31" s="35">
+        <v>0</v>
+      </c>
+      <c r="F31" s="35">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="G31" s="36" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C1" xr:uid="{125137E1-7B88-B544-BB44-BBBD3AC76342}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{125137E1-7B88-B544-BB44-BBBD3AC76342}">
       <formula1>DataLayouts</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C20" xr:uid="{12067159-7026-9D42-9AE3-5C0EBCF5C3E0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C31" xr:uid="{12067159-7026-9D42-9AE3-5C0EBCF5C3E0}">
       <formula1>_Streets</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D20" xr:uid="{183D1F80-CC1F-D341-A5C9-B55B214ED81E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D31" xr:uid="{183D1F80-CC1F-D341-A5C9-B55B214ED81E}">
       <formula1>_Actions</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:G5" xr:uid="{D439AD26-78D3-8049-B803-91FB77A799E5}">
@@ -3225,215 +4312,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E595855-FCC9-CD4F-A83B-9F0E43C081E7}">
-  <dimension ref="A1:F16"/>
-  <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="42.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="19.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6" s="2">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2">
-        <v>3</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" s="2">
-        <v>2</v>
-      </c>
-      <c r="C7" s="2">
-        <v>5</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B8" s="2">
-        <v>100</v>
-      </c>
-      <c r="C8" s="2">
-        <v>200</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E8" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="8"/>
-      <c r="C12" s="8"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="13"/>
-    </row>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{3AFABB3D-38C0-CA4B-96C5-C68C5E1F75DE}">
-      <formula1>DataLayouts</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:F5" xr:uid="{2B43068A-F86C-2F43-9DA6-BD346589A1EE}">
-      <formula1>TableDataTypes</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
 </file>
</xml_diff>